<commit_message>
finished zhugong card choosing
</commit_message>
<xml_diff>
--- a/data/data_core.xlsx
+++ b/data/data_core.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33912\PycharmProjects\SGS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BF8F2A-6145-46BB-B19A-73DEB1F1CF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95D1EA1-BFEE-4867-B8B2-B8F9482D7470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1400,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J320"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A291" workbookViewId="0">
+      <selection activeCell="O305" sqref="O305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1605,8 +1605,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
@@ -1857,7 +1856,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" ref="F12:F53" si="4">IF(E13=0,A13,"")</f>
+        <f t="shared" ref="F13:F53" si="4">IF(E13=0,A13,"")</f>
         <v>11</v>
       </c>
       <c r="G13" s="1">
@@ -1922,8 +1921,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -1994,8 +1992,7 @@
         <v>4</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
@@ -2102,8 +2099,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -2713,8 +2709,7 @@
         <v>4</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37" s="1">
         <v>0</v>
@@ -3610,8 +3605,7 @@
         <v>2</v>
       </c>
       <c r="D62" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E62" s="1">
         <v>0</v>
@@ -4687,8 +4681,7 @@
         <v>1</v>
       </c>
       <c r="D92" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E92" s="1">
         <v>0</v>
@@ -4759,8 +4752,7 @@
         <v>3</v>
       </c>
       <c r="D94" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E94" s="1">
         <v>0</v>
@@ -4903,8 +4895,7 @@
         <v>1</v>
       </c>
       <c r="D98" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98" s="1">
         <v>0</v>
@@ -4939,8 +4930,7 @@
         <v>2</v>
       </c>
       <c r="D99" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99" s="1">
         <v>0</v>
@@ -4975,8 +4965,7 @@
         <v>2</v>
       </c>
       <c r="D100" s="1">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100" s="1">
         <v>0</v>
@@ -6475,8 +6464,7 @@
         <v>4</v>
       </c>
       <c r="D142" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E142" s="1">
         <v>0</v>
@@ -6756,8 +6744,7 @@
         <v>3</v>
       </c>
       <c r="D150" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E150" s="1">
         <v>0</v>
@@ -7008,8 +6995,7 @@
         <v>2</v>
       </c>
       <c r="D157" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E157" s="1">
         <v>0</v>
@@ -8626,8 +8612,7 @@
         <v>3</v>
       </c>
       <c r="D202" s="1">
-        <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E202" s="1">
         <v>0</v>
@@ -8662,8 +8647,7 @@
         <v>3</v>
       </c>
       <c r="D203" s="1">
-        <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E203" s="1">
         <v>0</v>
@@ -10102,8 +10086,7 @@
         <v>2</v>
       </c>
       <c r="D243" s="1">
-        <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E243" s="1">
         <v>0</v>
@@ -10278,8 +10261,7 @@
         <v>1</v>
       </c>
       <c r="D248" s="1">
-        <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E248" s="1">
         <v>0</v>
@@ -10314,8 +10296,7 @@
         <v>1</v>
       </c>
       <c r="D249" s="1">
-        <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E249" s="1">
         <v>0</v>
@@ -11178,8 +11159,7 @@
         <v>2</v>
       </c>
       <c r="D273" s="1">
-        <f t="shared" si="19"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E273" s="1">
         <v>0</v>
@@ -11538,8 +11518,7 @@
         <v>2</v>
       </c>
       <c r="D283" s="1">
-        <f t="shared" si="19"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E283" s="1">
         <v>0</v>
@@ -11610,8 +11589,7 @@
         <v>2</v>
       </c>
       <c r="D285" s="1">
-        <f t="shared" si="19"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E285" s="1">
         <v>0</v>
@@ -12077,8 +12055,7 @@
         <v>2</v>
       </c>
       <c r="D298" s="1">
-        <f t="shared" si="19"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E298" s="1">
         <v>0</v>
@@ -12113,8 +12090,7 @@
         <v>2</v>
       </c>
       <c r="D299" s="1">
-        <f t="shared" si="19"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E299" s="1">
         <v>0</v>
@@ -12149,8 +12125,7 @@
         <v>2</v>
       </c>
       <c r="D300" s="1">
-        <f t="shared" si="19"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E300" s="1">
         <v>0</v>
@@ -12185,8 +12160,7 @@
         <v>1</v>
       </c>
       <c r="D301" s="1">
-        <f t="shared" si="19"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E301" s="1">
         <v>0</v>
@@ -12577,7 +12551,7 @@
         <v>4</v>
       </c>
       <c r="D312" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E312" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
added show pic function for 2*selector+2*base game
</commit_message>
<xml_diff>
--- a/data/data_core.xlsx
+++ b/data/data_core.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33912\PycharmProjects\SGS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0FC75D-49F5-4598-B429-DB50AB624212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934CEABD-B4C0-4521-89C1-73DB8E147EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="400" yWindow="400" windowWidth="19200" windowHeight="11180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1440,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="K196" sqref="K196"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1450,7 +1450,7 @@
     <col min="2" max="2" width="24.58203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.75" customWidth="1"/>
     <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
@@ -1855,7 +1855,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="1">
         <v>2</v>
@@ -6575,7 +6575,7 @@
         <v>4</v>
       </c>
       <c r="D144" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E144" s="1">
         <v>2</v>
@@ -8437,7 +8437,7 @@
         <v>2</v>
       </c>
       <c r="D196" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E196" s="1">
         <v>2</v>
@@ -12887,13 +12887,13 @@
         <v>329</v>
       </c>
       <c r="C321" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D321" s="1">
         <v>1</v>
       </c>
       <c r="E321" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F321" s="1">
         <v>319</v>
@@ -12909,7 +12909,7 @@
       </c>
       <c r="J321" s="1">
         <f t="shared" si="21"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="322" spans="1:10" ht="16.5" x14ac:dyDescent="0.45">
@@ -12926,7 +12926,7 @@
         <v>0</v>
       </c>
       <c r="E322" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F322" s="1">
         <v>319</v>
@@ -12942,7 +12942,7 @@
       </c>
       <c r="J322" s="1">
         <f t="shared" si="21"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="323" spans="1:10" ht="16.5" x14ac:dyDescent="0.45">

</xml_diff>